<commit_message>
Replace test case documents in readmeimages difrectory
</commit_message>
<xml_diff>
--- a/docs/readmeimages/racing-turtles_test-case-scenarios.xlsx
+++ b/docs/readmeimages/racing-turtles_test-case-scenarios.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="132">
   <si>
     <t>Test ID</t>
   </si>
@@ -1143,7 +1143,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1179,15 +1179,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1475,7 +1466,9 @@
       <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4">
@@ -1601,7 +1594,9 @@
       <c r="E9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10">
@@ -1620,7 +1615,9 @@
       <c r="E10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11">
@@ -1639,7 +1636,9 @@
       <c r="E11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G11" s="9"/>
     </row>
     <row r="12">
@@ -1658,7 +1657,9 @@
       <c r="E12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G12" s="9"/>
     </row>
     <row r="13">
@@ -1677,7 +1678,9 @@
       <c r="E13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G13" s="9"/>
     </row>
     <row r="14">
@@ -1759,7 +1762,9 @@
       <c r="E17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G17" s="11"/>
     </row>
     <row r="18">
@@ -1822,7 +1827,9 @@
       <c r="E20" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G20" s="8"/>
     </row>
     <row r="21">
@@ -1904,7 +1911,9 @@
       <c r="E24" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G24" s="9"/>
     </row>
     <row r="25">
@@ -1969,149 +1978,6 @@
         <v>12</v>
       </c>
       <c r="G27" s="9"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="4"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="4"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="4"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="9"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="4"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="9"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="4"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="9"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="4"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="9"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="4"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="4"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="4"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="9"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="4"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="9"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="9"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="9"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="12"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="9"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="12"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="9"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="12"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="9"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="4"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>